<commit_message>
TWG overview of NEON tools
</commit_message>
<xml_diff>
--- a/hbpSampling/subsampleSortExperiments/hbp_d1819_sortExperiment2021_data.xlsx
+++ b/hbpSampling/subsampleSortExperiments/hbp_d1819_sortExperiment2021_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pajaro/Documents/workDocuments/gitRepositories/neon-plant-sampling/hbpSampling/subsampleSortExperiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BAEB9D-1766-284F-8815-9F03BE496F8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D2EC3-1865-7344-A47C-0B4FE9DC316E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17780" yWindow="500" windowWidth="32300" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>clipID</t>
   </si>
@@ -155,6 +155,39 @@
         <scheme val="minor"/>
       </rPr>
       <t>(BRY from entire strip)</t>
+    </r>
+  </si>
+  <si>
+    <t>Data Sheet: D17 HBP sorting experiment for OSD from non-PG clip harvest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">subsampleFreshMass </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ALL - unsorted)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">subsampleDryMass </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OSD - sorted)</t>
     </r>
   </si>
 </sst>
@@ -494,6 +527,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -505,9 +541,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -837,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38130F8A-AF32-2B47-A3E7-9AEBC9BD4D56}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -862,18 +895,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" ht="46" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -882,7 +915,7 @@
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -923,9 +956,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="6">
-        <v>0.32</v>
-      </c>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
@@ -938,9 +969,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5">
-        <v>0.17</v>
-      </c>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
@@ -953,9 +982,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="5">
-        <v>0.14000000000000001</v>
-      </c>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
@@ -968,9 +995,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5">
-        <v>0.18</v>
-      </c>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
@@ -983,9 +1008,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5">
-        <v>0.14000000000000001</v>
-      </c>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
@@ -998,9 +1021,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5">
-        <v>0.06</v>
-      </c>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
@@ -1013,9 +1034,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5">
-        <v>0.28000000000000003</v>
-      </c>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
@@ -1028,9 +1047,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
@@ -1043,9 +1060,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
@@ -1058,9 +1073,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="5">
-        <v>0.11</v>
-      </c>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
@@ -1073,9 +1086,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5">
-        <v>0.04</v>
-      </c>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
@@ -1088,9 +1099,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5">
-        <v>0.11</v>
-      </c>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
@@ -1103,9 +1112,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="5">
-        <v>0.19</v>
-      </c>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
@@ -1118,9 +1125,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="5">
-        <v>0.16</v>
-      </c>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
@@ -1133,9 +1138,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5">
-        <v>0.28999999999999998</v>
-      </c>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
@@ -1148,9 +1151,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="5">
-        <v>0.16</v>
-      </c>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
@@ -1163,9 +1164,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5">
-        <v>1.25</v>
-      </c>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
@@ -1597,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1613,23 +1612,23 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="D2" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="D2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">

</xml_diff>